<commit_message>
Completed working security profile
</commit_message>
<xml_diff>
--- a/Data/FX effect elaborations.xlsx
+++ b/Data/FX effect elaborations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Y\Portfolio management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72DF346D-264B-4485-A509-09E862A4E4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE80BF-90CB-4D49-A2F3-3553EA949C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{FFA61786-FDD3-4E5E-9314-50713974019C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FFA61786-FDD3-4E5E-9314-50713974019C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Q</t>
   </si>
@@ -58,18 +58,83 @@
   </si>
   <si>
     <t>Buy-in P_FX</t>
+  </si>
+  <si>
+    <t>Based on UBSE</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Value (CHF)</t>
+  </si>
+  <si>
+    <t>Value (GBP)</t>
+  </si>
+  <si>
+    <t>BoP</t>
+  </si>
+  <si>
+    <t>Price appreciation</t>
+  </si>
+  <si>
+    <t>Price change</t>
+  </si>
+  <si>
+    <t>Cash in</t>
+  </si>
+  <si>
+    <t>EoP</t>
+  </si>
+  <si>
+    <t>P at purchase</t>
+  </si>
+  <si>
+    <t>P at period end</t>
+  </si>
+  <si>
+    <t>PA in foreign cur.</t>
+  </si>
+  <si>
+    <t>FX at period end</t>
+  </si>
+  <si>
+    <t>PA in base cur.</t>
+  </si>
+  <si>
+    <t>FX effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -93,13 +158,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,19 +485,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212FC7C3-6127-4D57-ACF8-E67F95D8E40D}">
-  <dimension ref="B3:Q9"/>
+  <dimension ref="A3:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I24" activeCellId="1" sqref="E34 I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="9.234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -461,7 +536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -499,7 +574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>+B4+1</f>
         <v>2</v>
@@ -538,7 +613,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>+B5+1</f>
         <v>3</v>
@@ -586,7 +661,7 @@
         <v>46.499999999999993</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G7">
         <f>SUM(G4:G6)</f>
         <v>20</v>
@@ -612,17 +687,415 @@
         <v>-22.5</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J8">
         <f>J7*(E6/E4-1)</f>
         <v>7.9999999999999982</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G9" s="3">
         <f>G7*(E6-E4)</f>
         <v>7.9999999999999982</v>
       </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>40179</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.6554</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>40424</v>
+      </c>
+      <c r="C18">
+        <v>18.09</v>
+      </c>
+      <c r="D18">
+        <v>270</v>
+      </c>
+      <c r="E18" s="2">
+        <f>C18*D18</f>
+        <v>4884.3</v>
+      </c>
+      <c r="F18">
+        <v>1.5591999999999999</v>
+      </c>
+      <c r="G18" s="2">
+        <f>E18/F18</f>
+        <v>3132.5679835813239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>E18/(D18+D19)</f>
+        <v>13.567500000000001</v>
+      </c>
+      <c r="B19" s="4">
+        <v>40425</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2">
+        <f>C19*D19</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1.5723</v>
+      </c>
+      <c r="G19" s="2">
+        <f>E19/F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>40543</v>
+      </c>
+      <c r="C21">
+        <v>15.35</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D17:D19)</f>
+        <v>360</v>
+      </c>
+      <c r="E21" s="2">
+        <f>C21*D21</f>
+        <v>5526</v>
+      </c>
+      <c r="F21">
+        <v>1.4575</v>
+      </c>
+      <c r="G21" s="2">
+        <f>E21/F21</f>
+        <v>3791.4236706689535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>41274</v>
+      </c>
+      <c r="C23">
+        <v>14.27</v>
+      </c>
+      <c r="D23">
+        <f>+D24</f>
+        <v>360</v>
+      </c>
+      <c r="E23" s="2">
+        <f>C23*D23</f>
+        <v>5137.2</v>
+      </c>
+      <c r="F23">
+        <v>1.4849000000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <f>E23/F23</f>
+        <v>3459.6269109030909</v>
+      </c>
+      <c r="I23">
+        <f>+D27*C23</f>
+        <v>4466.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>41275</v>
+      </c>
+      <c r="C24">
+        <v>14.27</v>
+      </c>
+      <c r="D24">
+        <v>360</v>
+      </c>
+      <c r="E24" s="2">
+        <f>C24*D24</f>
+        <v>5137.2</v>
+      </c>
+      <c r="F24">
+        <v>1.4849000000000001</v>
+      </c>
+      <c r="G24" s="2">
+        <f>E24/F24</f>
+        <v>3459.6269109030909</v>
+      </c>
+      <c r="I24" s="2">
+        <f>+E27-I23</f>
+        <v>829.45000000000073</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>41334</v>
+      </c>
+      <c r="C25">
+        <v>14.84</v>
+      </c>
+      <c r="D25">
+        <v>-47</v>
+      </c>
+      <c r="E25" s="2">
+        <f>C25*D25</f>
+        <v>-697.48</v>
+      </c>
+      <c r="F25">
+        <v>1.4278999999999999</v>
+      </c>
+      <c r="G25" s="2">
+        <f>E25/F25</f>
+        <v>-488.46557882204638</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>41639</v>
+      </c>
+      <c r="C27">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="D27">
+        <f>D24+D25</f>
+        <v>313</v>
+      </c>
+      <c r="E27" s="2">
+        <f>C27*D27</f>
+        <v>5295.9600000000009</v>
+      </c>
+      <c r="F27">
+        <v>1.4749000000000001</v>
+      </c>
+      <c r="G27" s="2">
+        <f>E27/F27</f>
+        <v>3590.7247949013495</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>D21</f>
+        <v>360</v>
+      </c>
+      <c r="E31">
+        <f>-D25</f>
+        <v>47</v>
+      </c>
+      <c r="F31">
+        <f>D27</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <f>+A19</f>
+        <v>13.567500000000001</v>
+      </c>
+      <c r="E32">
+        <f>C24</f>
+        <v>14.27</v>
+      </c>
+      <c r="F32">
+        <f>C24</f>
+        <v>14.27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <f>+C21</f>
+        <v>15.35</v>
+      </c>
+      <c r="E33">
+        <f>C25</f>
+        <v>14.84</v>
+      </c>
+      <c r="F33">
+        <f>C27</f>
+        <v>16.920000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <f>C31*(C33-C32)</f>
+        <v>641.69999999999959</v>
+      </c>
+      <c r="E34">
+        <f>E31*(E33-E32)</f>
+        <v>26.790000000000013</v>
+      </c>
+      <c r="F34">
+        <f>F31*(F33-F32)</f>
+        <v>829.45000000000061</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <f>F21</f>
+        <v>1.4575</v>
+      </c>
+      <c r="E35">
+        <f>F25</f>
+        <v>1.4278999999999999</v>
+      </c>
+      <c r="F35">
+        <f>+F27</f>
+        <v>1.4749000000000001</v>
+      </c>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="2">
+        <f>C34/C35</f>
+        <v>440.27444253859318</v>
+      </c>
+      <c r="E36" s="2">
+        <f>E34/E35</f>
+        <v>18.761818054485619</v>
+      </c>
+      <c r="F36" s="2">
+        <f>F34/F35</f>
+        <v>562.3771103125639</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="2">
+        <f>E39-E36</f>
+        <v>18.030247399657295</v>
+      </c>
+      <c r="F38" s="2">
+        <f>D27*C24/F24+F36-G27</f>
+        <v>-20.394287053597964</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E39" s="2">
+        <f>-G25+D25*C24/F24</f>
+        <v>36.792065454142914</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2">
+        <f>G17</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2">
+        <f>G18</f>
+        <v>3132.5679835813239</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="2">
+        <f>D21*(C21-A19)/F21</f>
+        <v>440.27444253859318</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <f>D21*A19*(1/F21-1/F18)</f>
+        <v>218.58124454903597</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="2">
+        <f>SUM(C44:C47)</f>
+        <v>3791.423670668953</v>
+      </c>
+      <c r="D48" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>